<commit_message>
fix expected fields for Edjin account creation
</commit_message>
<xml_diff>
--- a/docs/C5_provisioning-735-QA.xlsx
+++ b/docs/C5_provisioning-735-QA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scamus\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scamus\Projects\playground\edjin-node-provisioner\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838778DF-3E9E-4FE6-8398-0A51874053B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A3F90D-AAFF-4BF4-9367-F691C49A4385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$J$4</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="113">
   <si>
     <t>Password</t>
   </si>
@@ -45,9 +45,6 @@
     <t>State</t>
   </si>
   <si>
-    <t>Post Code</t>
-  </si>
-  <si>
     <t>User Role</t>
   </si>
   <si>
@@ -283,13 +280,100 @@
   </si>
   <si>
     <t>Lambert</t>
+  </si>
+  <si>
+    <t>Country Code</t>
+  </si>
+  <si>
+    <t>PH</t>
+  </si>
+  <si>
+    <t>UID</t>
+  </si>
+  <si>
+    <t>go5011782</t>
+  </si>
+  <si>
+    <t>go5011784</t>
+  </si>
+  <si>
+    <t>go5011783</t>
+  </si>
+  <si>
+    <t>07c9b69e-51b4-4443-9c91-16b06a7ced84</t>
+  </si>
+  <si>
+    <t>go5011785</t>
+  </si>
+  <si>
+    <t>go5011786</t>
+  </si>
+  <si>
+    <t>go5011787</t>
+  </si>
+  <si>
+    <t>go5011789</t>
+  </si>
+  <si>
+    <t>go5011788</t>
+  </si>
+  <si>
+    <t>go5011791</t>
+  </si>
+  <si>
+    <t>go5011790</t>
+  </si>
+  <si>
+    <t>go5011792</t>
+  </si>
+  <si>
+    <t>go5011794</t>
+  </si>
+  <si>
+    <t>go5011793</t>
+  </si>
+  <si>
+    <t>7c045c0d-db96-49c1-9276-95d9b07832bd</t>
+  </si>
+  <si>
+    <t>go5011795</t>
+  </si>
+  <si>
+    <t>go5011797</t>
+  </si>
+  <si>
+    <t>go5011796</t>
+  </si>
+  <si>
+    <t>go5011798</t>
+  </si>
+  <si>
+    <t>go5011799</t>
+  </si>
+  <si>
+    <t>go5011800</t>
+  </si>
+  <si>
+    <t>go5011801</t>
+  </si>
+  <si>
+    <t>go5011802</t>
+  </si>
+  <si>
+    <t>go5011803</t>
+  </si>
+  <si>
+    <t>go5011804</t>
+  </si>
+  <si>
+    <t>help496</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,6 +391,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -339,10 +430,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -624,102 +716,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y202"/>
+  <dimension ref="A1:Z202"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63.85546875" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
-    <col min="5" max="5" width="39.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="63.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="39.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    </row>
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
       <c r="H2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" t="s">
+    </row>
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>37</v>
-      </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" s="1"/>
+        <v>41</v>
+      </c>
+      <c r="E3" t="s">
+        <v>63</v>
+      </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K3" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="K3" t="s">
+        <v>37</v>
+      </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -734,33 +839,38 @@
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
-    </row>
-    <row r="4" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>37</v>
+      <c r="Z3" s="1"/>
+    </row>
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" s="1"/>
+        <v>42</v>
+      </c>
+      <c r="E4" t="s">
+        <v>64</v>
+      </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" t="s">
         <v>13</v>
       </c>
-      <c r="I4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -775,33 +885,38 @@
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
-    </row>
-    <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>37</v>
+      <c r="Z4" s="1"/>
+    </row>
+    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" s="1"/>
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
+        <v>64</v>
+      </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" t="s">
+        <v>85</v>
+      </c>
+      <c r="I5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" t="s">
         <v>13</v>
       </c>
-      <c r="I5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" t="s">
-        <v>14</v>
-      </c>
-      <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -816,33 +931,38 @@
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
-    </row>
-    <row r="6" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>37</v>
+      <c r="Z5" s="1"/>
+    </row>
+    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E6" s="1"/>
+        <v>43</v>
+      </c>
+      <c r="E6" t="s">
+        <v>65</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="I6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K6" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="K6" t="s">
+        <v>37</v>
+      </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
@@ -857,30 +977,35 @@
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
-    </row>
-    <row r="7" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>37</v>
+      <c r="Z6" s="1"/>
+    </row>
+    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E7" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="E7" t="s">
+        <v>66</v>
+      </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="I7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K7" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="J7" t="s">
+        <v>14</v>
+      </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
@@ -895,30 +1020,35 @@
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>37</v>
+      <c r="Z7" s="1"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E8" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="E8" t="s">
+        <v>67</v>
+      </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="I8" t="s">
-        <v>15</v>
-      </c>
-      <c r="K8" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="J8" t="s">
+        <v>14</v>
+      </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -933,432 +1063,550 @@
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="Z8" s="1"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" t="s">
+        <v>85</v>
+      </c>
+      <c r="I9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" t="s">
+        <v>85</v>
+      </c>
+      <c r="I10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" t="s">
         <v>37</v>
       </c>
-      <c r="C9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" t="s">
-        <v>69</v>
-      </c>
-      <c r="H9" t="s">
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11" t="s">
+        <v>85</v>
+      </c>
+      <c r="I11" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" t="s">
+        <v>71</v>
+      </c>
+      <c r="H12" t="s">
+        <v>85</v>
+      </c>
+      <c r="I12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" t="s">
         <v>13</v>
       </c>
-      <c r="I9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" t="s">
+        <v>72</v>
+      </c>
+      <c r="H13" t="s">
+        <v>85</v>
+      </c>
+      <c r="I13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J13" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13" t="s">
         <v>37</v>
       </c>
-      <c r="C10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" t="s">
-        <v>70</v>
-      </c>
-      <c r="H10" t="s">
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" t="s">
+        <v>73</v>
+      </c>
+      <c r="H14" t="s">
+        <v>85</v>
+      </c>
+      <c r="I14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" t="s">
+        <v>74</v>
+      </c>
+      <c r="H15" t="s">
+        <v>85</v>
+      </c>
+      <c r="I15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" t="s">
         <v>13</v>
       </c>
-      <c r="I10" t="s">
-        <v>15</v>
-      </c>
-      <c r="J10" t="s">
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" t="s">
+        <v>74</v>
+      </c>
+      <c r="H16" t="s">
+        <v>85</v>
+      </c>
+      <c r="I16" t="s">
+        <v>12</v>
+      </c>
+      <c r="J16" t="s">
+        <v>14</v>
+      </c>
+      <c r="K16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" t="s">
+        <v>75</v>
+      </c>
+      <c r="H17" t="s">
+        <v>85</v>
+      </c>
+      <c r="I17" t="s">
+        <v>12</v>
+      </c>
+      <c r="J17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" t="s">
+        <v>76</v>
+      </c>
+      <c r="H18" t="s">
+        <v>85</v>
+      </c>
+      <c r="I18" t="s">
+        <v>12</v>
+      </c>
+      <c r="J18" t="s">
+        <v>14</v>
+      </c>
+      <c r="K18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" t="s">
+        <v>77</v>
+      </c>
+      <c r="H19" t="s">
+        <v>85</v>
+      </c>
+      <c r="I19" t="s">
+        <v>12</v>
+      </c>
+      <c r="J19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" t="s">
+        <v>78</v>
+      </c>
+      <c r="H20" t="s">
+        <v>85</v>
+      </c>
+      <c r="I20" t="s">
+        <v>12</v>
+      </c>
+      <c r="J20" t="s">
+        <v>14</v>
+      </c>
+      <c r="K20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" t="s">
+        <v>79</v>
+      </c>
+      <c r="H21" t="s">
+        <v>85</v>
+      </c>
+      <c r="I21" t="s">
+        <v>12</v>
+      </c>
+      <c r="J21" t="s">
+        <v>14</v>
+      </c>
+      <c r="K21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" t="s">
+        <v>80</v>
+      </c>
+      <c r="H22" t="s">
+        <v>85</v>
+      </c>
+      <c r="I22" t="s">
+        <v>12</v>
+      </c>
+      <c r="J22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" t="s">
+        <v>80</v>
+      </c>
+      <c r="H23" t="s">
+        <v>85</v>
+      </c>
+      <c r="I23" t="s">
+        <v>12</v>
+      </c>
+      <c r="J23" t="s">
+        <v>14</v>
+      </c>
+      <c r="K23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="C24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" t="s">
+        <v>81</v>
+      </c>
+      <c r="H24" t="s">
+        <v>85</v>
+      </c>
+      <c r="I24" t="s">
+        <v>8</v>
+      </c>
+      <c r="J24" t="s">
+        <v>14</v>
+      </c>
+      <c r="K24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25" t="s">
+        <v>82</v>
+      </c>
+      <c r="H25" t="s">
+        <v>85</v>
+      </c>
+      <c r="I25" t="s">
+        <v>8</v>
+      </c>
+      <c r="J25" t="s">
         <v>37</v>
       </c>
-      <c r="C11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" t="s">
-        <v>71</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="K25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" t="s">
+        <v>83</v>
+      </c>
+      <c r="H26" t="s">
+        <v>85</v>
+      </c>
+      <c r="I26" t="s">
+        <v>8</v>
+      </c>
+      <c r="J26" t="s">
         <v>13</v>
       </c>
-      <c r="I11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" t="s">
-        <v>72</v>
-      </c>
-      <c r="H12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" t="s">
-        <v>73</v>
-      </c>
-      <c r="H13" t="s">
-        <v>13</v>
-      </c>
-      <c r="I13" t="s">
-        <v>15</v>
-      </c>
-      <c r="J13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" t="s">
-        <v>74</v>
-      </c>
-      <c r="H14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" t="s">
-        <v>75</v>
-      </c>
-      <c r="H15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I15" t="s">
-        <v>15</v>
-      </c>
-      <c r="J15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" t="s">
-        <v>75</v>
-      </c>
-      <c r="H16" t="s">
-        <v>13</v>
-      </c>
-      <c r="I16" t="s">
-        <v>15</v>
-      </c>
-      <c r="J16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" t="s">
-        <v>76</v>
-      </c>
-      <c r="H17" t="s">
-        <v>13</v>
-      </c>
-      <c r="I17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18" t="s">
-        <v>77</v>
-      </c>
-      <c r="H18" t="s">
-        <v>13</v>
-      </c>
-      <c r="I18" t="s">
-        <v>15</v>
-      </c>
-      <c r="J18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" t="s">
-        <v>78</v>
-      </c>
-      <c r="H19" t="s">
-        <v>13</v>
-      </c>
-      <c r="I19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D20" t="s">
-        <v>79</v>
-      </c>
-      <c r="H20" t="s">
-        <v>13</v>
-      </c>
-      <c r="I20" t="s">
-        <v>15</v>
-      </c>
-      <c r="J20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" t="s">
-        <v>58</v>
-      </c>
-      <c r="D21" t="s">
-        <v>80</v>
-      </c>
-      <c r="H21" t="s">
-        <v>13</v>
-      </c>
-      <c r="I21" t="s">
-        <v>15</v>
-      </c>
-      <c r="J21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22" t="s">
-        <v>81</v>
-      </c>
-      <c r="H22" t="s">
-        <v>13</v>
-      </c>
-      <c r="I22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" t="s">
-        <v>60</v>
-      </c>
-      <c r="D23" t="s">
-        <v>81</v>
-      </c>
-      <c r="H23" t="s">
-        <v>13</v>
-      </c>
-      <c r="I23" t="s">
-        <v>15</v>
-      </c>
-      <c r="J23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" t="s">
-        <v>61</v>
-      </c>
-      <c r="D24" t="s">
-        <v>82</v>
-      </c>
-      <c r="H24" t="s">
-        <v>9</v>
-      </c>
-      <c r="I24" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D25" t="s">
-        <v>83</v>
-      </c>
-      <c r="H25" t="s">
-        <v>9</v>
-      </c>
-      <c r="I25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" t="s">
-        <v>63</v>
-      </c>
-      <c r="D26" t="s">
-        <v>84</v>
-      </c>
-      <c r="H26" t="s">
-        <v>9</v>
-      </c>
-      <c r="I26" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="1"/>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A202" s="1"/>
+      <c r="K26" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B137" s="1"/>
+    </row>
+    <row r="202" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B202" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I4" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="B1:J4" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{1DB212C6-5203-44E2-87A2-6C1EAAAB82BD}"/>
-    <hyperlink ref="A3" r:id="rId2" display="mailto:pippa_calter_stg@pte-mailbox.cambridgedev.org" xr:uid="{79C2B502-7586-4A9F-B80B-2C1E6329E3B0}"/>
-    <hyperlink ref="A4" r:id="rId3" display="mailto:rachel_dolter_stg@pte-mailbox.cambridgedev.org" xr:uid="{20FCD08F-2154-4AAB-A9FB-B234F9AE06D9}"/>
-    <hyperlink ref="A5" r:id="rId4" display="mailto:rachel_dolter2_stg@pte-mailbox.cambridgedev.org" xr:uid="{804BD47A-C8F6-4935-AB00-0EC679C98937}"/>
-    <hyperlink ref="A6" r:id="rId5" display="mailto:sonia_dulter_stg@pte-mailbox.cambridgedev.org" xr:uid="{4FB11F9D-2467-4209-A055-A1172CDF51C8}"/>
-    <hyperlink ref="A7" r:id="rId6" display="mailto:sophie_gilter_stg@pte-mailbox.cambridgedev.org" xr:uid="{51E5204A-8A60-4720-A046-F2A7ECDC26B6}"/>
-    <hyperlink ref="A8" r:id="rId7" xr:uid="{67D2EA90-1117-4C2A-AAD7-B3A0D5C8FBA6}"/>
-    <hyperlink ref="A9" r:id="rId8" display="mailto:zoe_halter_stg@pte-mailbox.cambridgedev.org" xr:uid="{A3040AF0-4B61-4778-A5A6-5C97A16EE453}"/>
-    <hyperlink ref="A10" r:id="rId9" display="mailto:mary_wrlter_stg@pte-mailbox.cambridgedev.org" xr:uid="{C21C4DE9-9023-4CF6-8F0B-46F68310592E}"/>
-    <hyperlink ref="A11" r:id="rId10" display="mailto:megan_yolter_stg@pte-mailbox.cambridgedev.org" xr:uid="{B5541C3A-AFD8-4234-B315-06C6E3F52D66}"/>
-    <hyperlink ref="A12" r:id="rId11" display="mailto:caroline_valter_stg@pte-mailbox.cambridgedev.org" xr:uid="{5A96625B-8EC2-4FA7-8E89-B3AF84DCE269}"/>
-    <hyperlink ref="A13" r:id="rId12" display="mailto:austin_walter_stg@pte-mailbox.cambridgedev.org" xr:uid="{203FBA58-9733-4599-8952-2DEFA8760F3F}"/>
-    <hyperlink ref="A14" r:id="rId13" display="mailto:benjamin_talter_stg@pte-mailbox.cambridgedev.org" xr:uid="{002D43CE-23F4-40BE-84A1-CE22C1DB8644}"/>
-    <hyperlink ref="A15" r:id="rId14" display="mailto:colin_stlter_stg@pte-mailbox.cambridgedev.org" xr:uid="{F1ED2D2D-A3F0-403B-8D41-18F0E3EEB7FC}"/>
-    <hyperlink ref="A16" r:id="rId15" display="mailto:colin_stlter2_stg@pte-mailbox.cambridgedev.org" xr:uid="{D3837CE1-6AA9-465F-9436-1900D98F483F}"/>
-    <hyperlink ref="A17" r:id="rId16" display="mailto:connor_relter_stg@pte-mailbox.cambridgedev.org" xr:uid="{3691FB77-F907-46F6-BF8A-0856CE289F87}"/>
-    <hyperlink ref="A18" r:id="rId17" display="mailto:isaac_qulter_stg@pte-mailbox.cambridgedev.org" xr:uid="{41569F0A-D1E7-4C43-97B2-D0989F2B7BDC}"/>
-    <hyperlink ref="A19" r:id="rId18" display="mailto:jack_palter_stg@pte-mailbox.cambridgedev.org" xr:uid="{3483E1DA-73A2-490F-B44D-B0B08C9DD94A}"/>
-    <hyperlink ref="A20" r:id="rId19" display="mailto:justin_multer_stg@pte-mailbox.cambridgedev.org" xr:uid="{C7779505-C713-4B69-BEA1-00C4BDC6AAF3}"/>
-    <hyperlink ref="A21" r:id="rId20" display="mailto:keith_nalter_stg@pte-mailbox.cambridgedev.org" xr:uid="{80EB4D34-2A75-4DFD-BCFA-DC8CBA5CB4AB}"/>
-    <hyperlink ref="A22" r:id="rId21" display="mailto:victor_mclter_stg@pte-mailbox.cambridgedev.org" xr:uid="{13801B5F-13F8-4A33-9C9B-6966D6E20AA7}"/>
-    <hyperlink ref="A23" r:id="rId22" display="mailto:warren_mclter_stg@pte-mailbox.cambridgedev.org" xr:uid="{79286D42-03F0-4084-89CD-C2367212D404}"/>
-    <hyperlink ref="A24" r:id="rId23" display="mailto:kylie_gill_stg@pte-mailbox.cambridgedev.org" xr:uid="{E83FF14D-1F54-44E4-BC5A-31A473EFC526}"/>
-    <hyperlink ref="A25" r:id="rId24" display="mailto:lauren_knox_stg@pte-mailbox.cambridgedev.org" xr:uid="{4BE8ED61-13E0-42CD-BEE6-FE599AF90E32}"/>
-    <hyperlink ref="A26" r:id="rId25" display="mailto:max_lambert_stg@pte-mailbox.cambridgedev.org" xr:uid="{F2782F53-717C-497F-AFF6-2AEFFDB3534B}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{1DB212C6-5203-44E2-87A2-6C1EAAAB82BD}"/>
+    <hyperlink ref="B3" r:id="rId2" display="mailto:pippa_calter_stg@pte-mailbox.cambridgedev.org" xr:uid="{79C2B502-7586-4A9F-B80B-2C1E6329E3B0}"/>
+    <hyperlink ref="B4" r:id="rId3" display="mailto:rachel_dolter_stg@pte-mailbox.cambridgedev.org" xr:uid="{20FCD08F-2154-4AAB-A9FB-B234F9AE06D9}"/>
+    <hyperlink ref="B5" r:id="rId4" display="mailto:rachel_dolter2_stg@pte-mailbox.cambridgedev.org" xr:uid="{804BD47A-C8F6-4935-AB00-0EC679C98937}"/>
+    <hyperlink ref="B6" r:id="rId5" display="mailto:sonia_dulter_stg@pte-mailbox.cambridgedev.org" xr:uid="{4FB11F9D-2467-4209-A055-A1172CDF51C8}"/>
+    <hyperlink ref="B7" r:id="rId6" display="mailto:sophie_gilter_stg@pte-mailbox.cambridgedev.org" xr:uid="{51E5204A-8A60-4720-A046-F2A7ECDC26B6}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{67D2EA90-1117-4C2A-AAD7-B3A0D5C8FBA6}"/>
+    <hyperlink ref="B9" r:id="rId8" display="mailto:zoe_halter_stg@pte-mailbox.cambridgedev.org" xr:uid="{A3040AF0-4B61-4778-A5A6-5C97A16EE453}"/>
+    <hyperlink ref="B10" r:id="rId9" display="mailto:mary_wrlter_stg@pte-mailbox.cambridgedev.org" xr:uid="{C21C4DE9-9023-4CF6-8F0B-46F68310592E}"/>
+    <hyperlink ref="B11" r:id="rId10" display="mailto:megan_yolter_stg@pte-mailbox.cambridgedev.org" xr:uid="{B5541C3A-AFD8-4234-B315-06C6E3F52D66}"/>
+    <hyperlink ref="B12" r:id="rId11" display="mailto:caroline_valter_stg@pte-mailbox.cambridgedev.org" xr:uid="{5A96625B-8EC2-4FA7-8E89-B3AF84DCE269}"/>
+    <hyperlink ref="B13" r:id="rId12" display="mailto:austin_walter_stg@pte-mailbox.cambridgedev.org" xr:uid="{203FBA58-9733-4599-8952-2DEFA8760F3F}"/>
+    <hyperlink ref="B14" r:id="rId13" display="mailto:benjamin_talter_stg@pte-mailbox.cambridgedev.org" xr:uid="{002D43CE-23F4-40BE-84A1-CE22C1DB8644}"/>
+    <hyperlink ref="B15" r:id="rId14" display="mailto:colin_stlter_stg@pte-mailbox.cambridgedev.org" xr:uid="{F1ED2D2D-A3F0-403B-8D41-18F0E3EEB7FC}"/>
+    <hyperlink ref="B16" r:id="rId15" display="mailto:colin_stlter2_stg@pte-mailbox.cambridgedev.org" xr:uid="{D3837CE1-6AA9-465F-9436-1900D98F483F}"/>
+    <hyperlink ref="B17" r:id="rId16" display="mailto:connor_relter_stg@pte-mailbox.cambridgedev.org" xr:uid="{3691FB77-F907-46F6-BF8A-0856CE289F87}"/>
+    <hyperlink ref="B18" r:id="rId17" display="mailto:isaac_qulter_stg@pte-mailbox.cambridgedev.org" xr:uid="{41569F0A-D1E7-4C43-97B2-D0989F2B7BDC}"/>
+    <hyperlink ref="B19" r:id="rId18" display="mailto:jack_palter_stg@pte-mailbox.cambridgedev.org" xr:uid="{3483E1DA-73A2-490F-B44D-B0B08C9DD94A}"/>
+    <hyperlink ref="B20" r:id="rId19" display="mailto:justin_multer_stg@pte-mailbox.cambridgedev.org" xr:uid="{C7779505-C713-4B69-BEA1-00C4BDC6AAF3}"/>
+    <hyperlink ref="B21" r:id="rId20" display="mailto:keith_nalter_stg@pte-mailbox.cambridgedev.org" xr:uid="{80EB4D34-2A75-4DFD-BCFA-DC8CBA5CB4AB}"/>
+    <hyperlink ref="B22" r:id="rId21" display="mailto:victor_mclter_stg@pte-mailbox.cambridgedev.org" xr:uid="{13801B5F-13F8-4A33-9C9B-6966D6E20AA7}"/>
+    <hyperlink ref="B23" r:id="rId22" display="mailto:warren_mclter_stg@pte-mailbox.cambridgedev.org" xr:uid="{79286D42-03F0-4084-89CD-C2367212D404}"/>
+    <hyperlink ref="B24" r:id="rId23" display="mailto:kylie_gill_stg@pte-mailbox.cambridgedev.org" xr:uid="{E83FF14D-1F54-44E4-BC5A-31A473EFC526}"/>
+    <hyperlink ref="B25" r:id="rId24" display="mailto:lauren_knox_stg@pte-mailbox.cambridgedev.org" xr:uid="{4BE8ED61-13E0-42CD-BEE6-FE599AF90E32}"/>
+    <hyperlink ref="B26" r:id="rId25" display="mailto:max_lambert_stg@pte-mailbox.cambridgedev.org" xr:uid="{F2782F53-717C-497F-AFF6-2AEFFDB3534B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId26"/>
@@ -1366,15 +1614,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -1382,6 +1621,15 @@
     <_Flow_SignoffStatus xmlns="4aec70d8-0f38-47bb-bdd9-41e9e539b503" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1572,14 +1820,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{88ACEE29-6E32-4774-B795-1485D120139C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{917BA34E-18B2-45AE-9834-35B06F928D1E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -1592,6 +1832,14 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{88ACEE29-6E32-4774-B795-1485D120139C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
ILAMATHS-210 finalized status reporting and added some refactoring. created excelToJson script for other potential uses
</commit_message>
<xml_diff>
--- a/docs/C5_provisioning-735-QA.xlsx
+++ b/docs/C5_provisioning-735-QA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\cambridge\kc\edjin-node-provisioner\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6260DCEE-EF04-4B4F-BC2C-4348974A3327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9309F55-80C7-49FB-8E6E-ADFCE1D51E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,12 +69,6 @@
     <t>Student</t>
   </si>
   <si>
-    <t>broth151</t>
-  </si>
-  <si>
-    <t>soon227</t>
-  </si>
-  <si>
     <t>pippa_calter_stg@pte-mailbox.cambridgedev.org</t>
   </si>
   <si>
@@ -363,9 +357,6 @@
     <t>go5011804</t>
   </si>
   <si>
-    <t>help496</t>
-  </si>
-  <si>
     <t>julian_griffin@pte-mailbox.cambridgedev.org</t>
   </si>
   <si>
@@ -466,6 +457,15 @@
   </si>
   <si>
     <t>AU</t>
+  </si>
+  <si>
+    <t>stunt135</t>
+  </si>
+  <si>
+    <t>gone498</t>
+  </si>
+  <si>
+    <t>chomp997</t>
   </si>
 </sst>
 </file>
@@ -827,7 +827,7 @@
   <dimension ref="A1:Z202"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,12 +840,13 @@
     <col min="6" max="6" width="39.7109375" customWidth="1"/>
     <col min="8" max="8" width="15.140625" customWidth="1"/>
     <col min="9" max="9" width="17.85546875" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
@@ -866,7 +867,7 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
@@ -877,13 +878,13 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -892,19 +893,19 @@
         <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I2" t="s">
         <v>12</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>13</v>
+        <v>144</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="M2" s="11"/>
       <c r="N2" s="11"/>
@@ -912,39 +913,39 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="11" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I3" t="s">
         <v>12</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="L3" s="11" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="N3" s="12"/>
       <c r="O3" s="12"/>
@@ -962,42 +963,42 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="11" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I4" t="s">
         <v>12</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>13</v>
+        <v>144</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="N4" s="11" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="O4" s="12"/>
       <c r="P4" s="1"/>
@@ -1014,42 +1015,42 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="11" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I5" t="s">
         <v>12</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>13</v>
+        <v>144</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="N5" s="11" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="O5" s="12"/>
       <c r="P5" s="1"/>
@@ -1066,45 +1067,45 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="11" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I6" t="s">
         <v>12</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="L6" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="O6" s="11" t="s">
         <v>124</v>
-      </c>
-      <c r="M6" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="N6" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="O6" s="11" t="s">
-        <v>127</v>
       </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
@@ -1120,36 +1121,36 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="11" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I7" t="s">
         <v>12</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="K7" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L7" s="11" t="s">
         <v>124</v>
-      </c>
-      <c r="L7" s="11" t="s">
-        <v>127</v>
       </c>
       <c r="M7" s="12"/>
       <c r="N7" s="12"/>
@@ -1168,36 +1169,36 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="11" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I8" t="s">
         <v>12</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="M8" s="12"/>
       <c r="N8" s="12"/>
@@ -1216,105 +1217,105 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I9" t="s">
         <v>12</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>13</v>
+        <v>144</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="N9" s="11"/>
       <c r="O9" s="11"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I10" t="s">
         <v>12</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="M10" s="11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="N10" s="11"/>
       <c r="O10" s="11"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I11" t="s">
         <v>12</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="L11" s="11"/>
       <c r="M11" s="11"/>
@@ -1323,31 +1324,31 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H12" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I12" t="s">
         <v>12</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>13</v>
+        <v>144</v>
       </c>
       <c r="L12" s="11"/>
       <c r="M12" s="11"/>
@@ -1356,34 +1357,34 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I13" t="s">
         <v>12</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="L13" s="11" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="M13" s="11"/>
       <c r="N13" s="11"/>
@@ -1391,34 +1392,34 @@
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I14" t="s">
         <v>12</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="K14" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L14" s="11" t="s">
         <v>124</v>
-      </c>
-      <c r="L14" s="11" t="s">
-        <v>127</v>
       </c>
       <c r="M14" s="11"/>
       <c r="N14" s="11"/>
@@ -1426,108 +1427,108 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I15" t="s">
         <v>12</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>13</v>
+        <v>144</v>
       </c>
       <c r="L15" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="M15" s="11" t="s">
         <v>124</v>
-      </c>
-      <c r="M15" s="11" t="s">
-        <v>127</v>
       </c>
       <c r="N15" s="11"/>
       <c r="O15" s="11"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I16" t="s">
         <v>12</v>
       </c>
       <c r="J16" s="11" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="K16" s="11" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="L16" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="M16" s="11" t="s">
         <v>124</v>
-      </c>
-      <c r="M16" s="11" t="s">
-        <v>127</v>
       </c>
       <c r="N16" s="11"/>
       <c r="O16" s="11"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I17" t="s">
         <v>12</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="L17" s="11" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="M17" s="11"/>
       <c r="N17" s="11"/>
@@ -1535,71 +1536,71 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I18" t="s">
         <v>12</v>
       </c>
       <c r="J18" s="11" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>13</v>
+        <v>144</v>
       </c>
       <c r="L18" s="11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="M18" s="11" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="N18" s="11"/>
       <c r="O18" s="11"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I19" t="s">
         <v>12</v>
       </c>
       <c r="J19" s="11" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="L19" s="11" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="M19" s="11"/>
       <c r="N19" s="11"/>
@@ -1607,34 +1608,34 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E20" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I20" t="s">
         <v>12</v>
       </c>
       <c r="J20" s="11" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="K20" s="11" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="L20" s="11" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="M20" s="11"/>
       <c r="N20" s="11"/>
@@ -1642,31 +1643,31 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I21" s="9" t="s">
         <v>12</v>
       </c>
       <c r="J21" s="11" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="K21" s="11" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="L21" s="11"/>
       <c r="M21" s="11"/>
@@ -1675,147 +1676,147 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I22" s="9" t="s">
         <v>12</v>
       </c>
       <c r="J22" s="11" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="K22" s="11" t="s">
-        <v>13</v>
+        <v>144</v>
       </c>
       <c r="L22" s="11" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="M22" s="11" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="N22" s="11"/>
       <c r="O22" s="11"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I23" s="9" t="s">
         <v>12</v>
       </c>
       <c r="J23" s="11" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="K23" s="11" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="L23" s="11" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="M23" s="11" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="N23" s="11"/>
       <c r="O23" s="11"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E24" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H24" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I24" t="s">
         <v>12</v>
       </c>
       <c r="J24" s="11" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="K24" s="11" t="s">
-        <v>13</v>
+        <v>144</v>
       </c>
       <c r="L24" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="M24" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="N24" s="11" t="s">
         <v>124</v>
-      </c>
-      <c r="M24" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="N24" s="11" t="s">
-        <v>127</v>
       </c>
       <c r="O24" s="11"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E25" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H25" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I25" t="s">
         <v>12</v>
       </c>
       <c r="J25" s="11" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="K25" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L25" s="11" t="s">
         <v>124</v>
-      </c>
-      <c r="L25" s="11" t="s">
-        <v>127</v>
       </c>
       <c r="M25" s="11"/>
       <c r="N25" s="11"/>
@@ -1823,296 +1824,296 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D26" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I26" t="s">
         <v>12</v>
       </c>
       <c r="J26" s="11" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="K26" s="11" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="L26" s="11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="M26" s="11" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="N26" s="11"/>
       <c r="O26" s="11"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E27" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I27" t="s">
         <v>8</v>
       </c>
       <c r="J27" s="8" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="K27" s="8" t="s">
-        <v>13</v>
+        <v>144</v>
       </c>
       <c r="L27" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="M27" s="8" t="s">
         <v>124</v>
-      </c>
-      <c r="M27" s="8" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C28" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E28" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H28" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I28" t="s">
         <v>8</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="K28" s="8" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="M28" s="8" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C29" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E29" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I29" t="s">
         <v>8</v>
       </c>
       <c r="J29" s="8" t="s">
-        <v>13</v>
+        <v>144</v>
       </c>
       <c r="K29" s="8" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="L29" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="M29" s="8" t="s">
         <v>124</v>
-      </c>
-      <c r="M29" s="8" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="H30" t="s">
         <v>140</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="H30" t="s">
-        <v>143</v>
       </c>
       <c r="I30" s="6" t="s">
         <v>8</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>13</v>
+        <v>144</v>
       </c>
       <c r="K30" s="7" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="L30" s="7" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="M30" s="7" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="N30" s="7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="O30" s="7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="H31" t="s">
         <v>141</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="H31" t="s">
-        <v>144</v>
       </c>
       <c r="I31" s="6" t="s">
         <v>8</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>13</v>
+        <v>144</v>
       </c>
       <c r="K31" s="7" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="L31" s="7" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="M31" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="N31" s="7" t="s">
         <v>124</v>
-      </c>
-      <c r="N31" s="7" t="s">
-        <v>127</v>
       </c>
       <c r="O31" s="7"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H32" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I32" s="6" t="s">
         <v>8</v>
       </c>
       <c r="J32" s="7" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="K32" s="7" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="L32" s="7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="M32" s="7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="N32" s="7"/>
       <c r="O32" s="7"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="H33" t="s">
         <v>142</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="H33" t="s">
-        <v>145</v>
       </c>
       <c r="I33" s="6" t="s">
         <v>8</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>13</v>
+        <v>144</v>
       </c>
       <c r="K33" s="7" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="L33" s="7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="M33" s="7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="137" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>